<commit_message>
Adicionado a 3 página no projeto com visual diferente
Adicionado a 3 página no projeto com visual diferente
</commit_message>
<xml_diff>
--- a/PrecificarEquipamentos_Duda.xlsx
+++ b/PrecificarEquipamentos_Duda.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26516"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://oceanpact.sharepoint.com/sites/Projetoinventrio/Documentos Compartilhados/General/INVENTÁRIO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://oceanpact-my.sharepoint.com/personal/william_silva_oceanpact_com/Documents/Documentos/GitHub/Inventario_PowerBI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1087" documentId="8_{72529B7D-A18F-4E0A-9CAE-0F418ECF5B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB8551A7-1C26-4570-9EC6-B0E27E9C72D0}"/>
+  <xr:revisionPtr revIDLastSave="1093" documentId="8_{72529B7D-A18F-4E0A-9CAE-0F418ECF5B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DE5AB63-0184-42DB-A814-C340A1F792AA}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2964" yWindow="2964" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Duda" sheetId="1" r:id="rId1"/>
@@ -44,41 +44,41 @@
   <commentList>
     <comment ref="M109" authorId="0" shapeId="0" xr:uid="{9B39A4C3-88EB-4E72-B6CE-44FFDA3D7AAA}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentário encadeado]
+Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
+Comentário:
     Confirmar amanhã</t>
       </text>
     </comment>
     <comment ref="M110" authorId="1" shapeId="0" xr:uid="{50C4091B-4129-43C8-B8AF-A76D2B356C49}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentário encadeado]
+Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
+Comentário:
     Inoperante</t>
       </text>
     </comment>
     <comment ref="M130" authorId="2" shapeId="0" xr:uid="{481D60E5-DC93-4F5B-95A7-B615FADBFA37}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentário encadeado]
+Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
+Comentário:
     Inoperante</t>
       </text>
     </comment>
     <comment ref="H140" authorId="3" shapeId="0" xr:uid="{133877F9-B89D-4F9F-A48D-A9FE089DC91C}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentário encadeado]
+Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
+Comentário:
     Tem 3, mas todas estão ruins</t>
       </text>
     </comment>
     <comment ref="H141" authorId="4" shapeId="0" xr:uid="{E8FEC7E3-B860-4E63-83C5-C5874548E571}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentário encadeado]
+Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
+Comentário:
     Tem 3, mas todas estão ruins</t>
       </text>
     </comment>
@@ -2050,7 +2050,7 @@
     <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3711,13 +3711,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -3736,6 +3729,13 @@
       <fill>
         <patternFill patternType="none"/>
       </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -3950,20 +3950,20 @@
     <v>5</v>
     <v>5.5297000000000001</v>
     <v>4.6896000000000004</v>
-    <v>4.9762000000000004</v>
-    <v>4.9352</v>
+    <v>4.9926000000000004</v>
+    <v>4.9424999999999999</v>
     <v>USD</v>
-    <v>4.9714</v>
-    <v>45070.757997685185</v>
+    <v>4.9619</v>
+    <v>45071.55537037037</v>
     <v>BRL</v>
     <v>US Dollar/Brazilian Real FX Spot Rate</v>
-    <v>4.9714</v>
-    <v>4.9469000000000003</v>
+    <v>4.9610000000000003</v>
+    <v>4.9873000000000003</v>
     <v>USDBRL</v>
     <v>Par de Moedas</v>
     <v>USD/BRL</v>
-    <v>-2.4500000000000001E-2</v>
-    <v>-4.9280000000000001E-3</v>
+    <v>2.5399999999999999E-2</v>
+    <v>5.1190000000000003E-3</v>
   </rv>
   <rv s="1">
     <v>0</v>
@@ -4188,7 +4188,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{487EB123-9A0E-4DE6-AC09-2D80046E6087}" name="Tabela1" displayName="Tabela1" ref="A1:I281" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{487EB123-9A0E-4DE6-AC09-2D80046E6087}" name="Tabela1" displayName="Tabela1" ref="A1:I281" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="A1:I281" xr:uid="{487EB123-9A0E-4DE6-AC09-2D80046E6087}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{3DB87A71-FCE0-4F2B-8162-CE1B89AB53E9}" name="FIRME?" dataDxfId="8"/>
@@ -4206,7 +4206,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4525,24 +4525,24 @@
   <dimension ref="A1:XFB282"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E246" sqref="E246"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.28515625" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" style="8" customWidth="1"/>
-    <col min="6" max="7" width="24.85546875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="58.33203125" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" style="8" customWidth="1"/>
+    <col min="6" max="7" width="24.88671875" style="7" customWidth="1"/>
     <col min="8" max="8" width="19" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="172.5703125" customWidth="1"/>
-    <col min="10" max="12" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="172.5546875" customWidth="1"/>
+    <col min="10" max="12" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21.6" thickBot="1">
+    <row r="1" spans="1:13" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -4575,7 +4575,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15" thickBot="1">
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>10</v>
       </c>
@@ -4593,7 +4593,7 @@
       </c>
       <c r="F2" s="22">
         <f>E2*K2</f>
-        <v>204653.25300000003</v>
+        <v>206324.60100000002</v>
       </c>
       <c r="G2" s="22"/>
       <c r="H2" s="11">
@@ -4607,14 +4607,14 @@
       </c>
       <c r="K2" s="2" cm="1">
         <f t="array" ref="K2">_FV(J2,"Preço",TRUE)</f>
-        <v>4.9469000000000003</v>
+        <v>4.9873000000000003</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1">
+    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -4632,7 +4632,7 @@
       </c>
       <c r="F3" s="22">
         <f>E3*K2</f>
-        <v>204653.25300000003</v>
+        <v>206324.60100000002</v>
       </c>
       <c r="G3" s="22"/>
       <c r="H3" s="11">
@@ -4647,7 +4647,7 @@
       </c>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>10</v>
       </c>
@@ -4665,7 +4665,7 @@
       </c>
       <c r="F4" s="22">
         <f>E4*K2</f>
-        <v>204653.25300000003</v>
+        <v>206324.60100000002</v>
       </c>
       <c r="G4" s="22"/>
       <c r="H4" s="11">
@@ -4674,7 +4674,7 @@
       <c r="I4" s="12"/>
       <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>19</v>
       </c>
@@ -4693,7 +4693,7 @@
       </c>
       <c r="F5" s="22">
         <f>K2*E5</f>
-        <v>129984.74440000001</v>
+        <v>131046.2948</v>
       </c>
       <c r="G5" s="22"/>
       <c r="H5" s="11">
@@ -4707,7 +4707,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>19</v>
       </c>
@@ -4726,7 +4726,7 @@
       </c>
       <c r="F6" s="22">
         <f>K2*E6</f>
-        <v>154719.2444</v>
+        <v>155982.7948</v>
       </c>
       <c r="G6" s="22"/>
       <c r="H6" s="10">
@@ -4740,7 +4740,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>19</v>
       </c>
@@ -4758,7 +4758,7 @@
       </c>
       <c r="F7" s="22">
         <f>K2*E7</f>
-        <v>139878.54440000001</v>
+        <v>141020.89480000001</v>
       </c>
       <c r="G7" s="22"/>
       <c r="H7" s="10">
@@ -4772,7 +4772,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>10</v>
       </c>
@@ -4790,7 +4790,7 @@
       </c>
       <c r="F8" s="22">
         <f>K2*E8</f>
-        <v>267206.20987199998</v>
+        <v>269388.41102400003</v>
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="11">
@@ -4804,7 +4804,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
@@ -4822,7 +4822,7 @@
       </c>
       <c r="F9" s="22">
         <f>K2*E9</f>
-        <v>100669.41500000001</v>
+        <v>101491.55500000001</v>
       </c>
       <c r="G9" s="22"/>
       <c r="H9" s="10">
@@ -4836,7 +4836,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>10</v>
       </c>
@@ -4854,7 +4854,7 @@
       </c>
       <c r="F10" s="22">
         <f>K2*E10</f>
-        <v>160361.23331899999</v>
+        <v>161670.860323</v>
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="10">
@@ -4868,7 +4868,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15" customHeight="1">
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
@@ -4886,7 +4886,7 @@
       </c>
       <c r="F11" s="22">
         <f>K2*E11</f>
-        <v>380777.73370000004</v>
+        <v>383887.44290000002</v>
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="10">
@@ -4900,7 +4900,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>19</v>
       </c>
@@ -4918,7 +4918,7 @@
       </c>
       <c r="F12" s="22">
         <f>K2*E12</f>
-        <v>118725.6</v>
+        <v>119695.20000000001</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="10">
@@ -4932,7 +4932,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1">
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>10</v>
       </c>
@@ -4950,7 +4950,7 @@
       </c>
       <c r="F13" s="22">
         <f>K2*E13</f>
-        <v>167289.31730000002</v>
+        <v>168655.52410000001</v>
       </c>
       <c r="G13" s="22"/>
       <c r="H13" s="10">
@@ -4965,7 +4965,7 @@
       <c r="K13" s="106"/>
       <c r="L13" s="106"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>10</v>
       </c>
@@ -4983,7 +4983,7 @@
       </c>
       <c r="F14" s="22">
         <f>K2*E14</f>
-        <v>167289.31730000002</v>
+        <v>168655.52410000001</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="10">
@@ -4998,7 +4998,7 @@
       <c r="K14" s="106"/>
       <c r="L14" s="106"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="10" t="s">
         <v>43</v>
@@ -5014,7 +5014,7 @@
       </c>
       <c r="F15" s="22">
         <f>K2*E15</f>
-        <v>1166.528489</v>
+        <v>1176.0552130000001</v>
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="10">
@@ -5028,7 +5028,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" s="10" t="s">
         <v>46</v>
@@ -5044,7 +5044,7 @@
       </c>
       <c r="F16" s="22">
         <f>K2*E16</f>
-        <v>34380.955000000002</v>
+        <v>34661.735000000001</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="10">
@@ -5058,7 +5058,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
       <c r="B17" s="10" t="s">
         <v>46</v>
@@ -5074,7 +5074,7 @@
       </c>
       <c r="F17" s="22">
         <f>K2*E17</f>
-        <v>25352.862500000003</v>
+        <v>25559.912500000002</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="10">
@@ -5088,7 +5088,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="10" t="s">
         <v>46</v>
@@ -5104,7 +5104,7 @@
       </c>
       <c r="F18" s="22">
         <f>K2*E18</f>
-        <v>34380.955000000002</v>
+        <v>34661.735000000001</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="10">
@@ -5118,7 +5118,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15" customHeight="1">
+    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>10</v>
       </c>
@@ -5136,7 +5136,7 @@
       </c>
       <c r="F19" s="22">
         <f>K2*E19</f>
-        <v>2147.3503519999999</v>
+        <v>2164.8871840000002</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="10">
@@ -5150,7 +5150,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>10</v>
       </c>
@@ -5168,7 +5168,7 @@
       </c>
       <c r="F20" s="22">
         <f>K2*E20</f>
-        <v>2147.3503519999999</v>
+        <v>2164.8871840000002</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="10">
@@ -5182,7 +5182,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>10</v>
       </c>
@@ -5200,7 +5200,7 @@
       </c>
       <c r="F21" s="22">
         <f>K2*E21</f>
-        <v>2147.3503519999999</v>
+        <v>2164.8871840000002</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="11">
@@ -5214,7 +5214,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>10</v>
       </c>
@@ -5232,7 +5232,7 @@
       </c>
       <c r="F22" s="22">
         <f>K2*E22</f>
-        <v>2147.3503519999999</v>
+        <v>2164.8871840000002</v>
       </c>
       <c r="G22" s="22"/>
       <c r="H22" s="10">
@@ -5246,7 +5246,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
       <c r="B23" s="10" t="s">
         <v>60</v>
@@ -5262,7 +5262,7 @@
       </c>
       <c r="F23" s="22">
         <f>K2*E23</f>
-        <v>9893.8000000000011</v>
+        <v>9974.6</v>
       </c>
       <c r="G23" s="22"/>
       <c r="H23" s="10">
@@ -5276,7 +5276,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="9"/>
       <c r="B24" s="10" t="s">
         <v>60</v>
@@ -5292,7 +5292,7 @@
       </c>
       <c r="F24" s="22">
         <f>K2*E24</f>
-        <v>9893.8000000000011</v>
+        <v>9974.6</v>
       </c>
       <c r="G24" s="22"/>
       <c r="H24" s="10">
@@ -5306,7 +5306,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15" customHeight="1">
+    <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
       <c r="B25" s="10" t="s">
         <v>60</v>
@@ -5322,7 +5322,7 @@
       </c>
       <c r="F25" s="22">
         <f>K2*E25</f>
-        <v>9893.8000000000011</v>
+        <v>9974.6</v>
       </c>
       <c r="G25" s="22"/>
       <c r="H25" s="10">
@@ -5336,7 +5336,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
       <c r="B26" s="10" t="s">
         <v>60</v>
@@ -5352,7 +5352,7 @@
       </c>
       <c r="F26" s="22">
         <f>K2*E26</f>
-        <v>4843.0151000000005</v>
+        <v>4882.5667000000003</v>
       </c>
       <c r="G26" s="22"/>
       <c r="H26" s="10">
@@ -5366,7 +5366,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>10</v>
       </c>
@@ -5384,7 +5384,7 @@
       </c>
       <c r="F27" s="22">
         <f>K2*E27</f>
-        <v>75288.355169999995</v>
+        <v>75903.214890000003</v>
       </c>
       <c r="G27" s="22"/>
       <c r="H27" s="11">
@@ -5398,7 +5398,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="14.45" customHeight="1">
+    <row r="28" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>10</v>
       </c>
@@ -5416,7 +5416,7 @@
       </c>
       <c r="F28" s="22">
         <f>K2*E28</f>
-        <v>54415.9</v>
+        <v>54860.3</v>
       </c>
       <c r="G28" s="22"/>
       <c r="H28" s="10">
@@ -5431,7 +5431,7 @@
       <c r="K28" s="106"/>
       <c r="L28" s="106"/>
     </row>
-    <row r="29" spans="1:12" ht="15" customHeight="1">
+    <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>10</v>
       </c>
@@ -5449,7 +5449,7 @@
       </c>
       <c r="F29" s="22">
         <f>K2*E29</f>
-        <v>54415.9</v>
+        <v>54860.3</v>
       </c>
       <c r="G29" s="22"/>
       <c r="H29" s="11">
@@ -5464,7 +5464,7 @@
       <c r="K29" s="106"/>
       <c r="L29" s="106"/>
     </row>
-    <row r="30" spans="1:12" ht="15" customHeight="1">
+    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>19</v>
       </c>
@@ -5482,7 +5482,7 @@
       </c>
       <c r="F30" s="22">
         <f>K$2*E30</f>
-        <v>89044.200000000012</v>
+        <v>89771.400000000009</v>
       </c>
       <c r="G30" s="22"/>
       <c r="H30" s="10">
@@ -5495,7 +5495,7 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>19</v>
       </c>
@@ -5513,7 +5513,7 @@
       </c>
       <c r="F31" s="22">
         <f>K2*E31</f>
-        <v>24734.5</v>
+        <v>24936.5</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="11">
@@ -5526,7 +5526,7 @@
       <c r="K31" s="106"/>
       <c r="L31" s="106"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>19</v>
       </c>
@@ -5544,7 +5544,7 @@
       </c>
       <c r="F32" s="22">
         <f>K2*E32</f>
-        <v>3284.7416000000003</v>
+        <v>3311.5672000000004</v>
       </c>
       <c r="G32" s="22"/>
       <c r="H32" s="10">
@@ -5558,7 +5558,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>19</v>
       </c>
@@ -5576,7 +5576,7 @@
       </c>
       <c r="F33" s="22">
         <f>K2*E33</f>
-        <v>3284.7416000000003</v>
+        <v>3311.5672000000004</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="11">
@@ -5590,7 +5590,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>19</v>
       </c>
@@ -5608,7 +5608,7 @@
       </c>
       <c r="F34" s="22">
         <f>K2*E34</f>
-        <v>3284.7416000000003</v>
+        <v>3311.5672000000004</v>
       </c>
       <c r="G34" s="22"/>
       <c r="H34" s="10">
@@ -5622,7 +5622,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
         <v>19</v>
       </c>
@@ -5640,7 +5640,7 @@
       </c>
       <c r="F35" s="22">
         <f>K2*E35</f>
-        <v>3284.7416000000003</v>
+        <v>3311.5672000000004</v>
       </c>
       <c r="G35" s="22"/>
       <c r="H35" s="10">
@@ -5654,7 +5654,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
         <v>86</v>
@@ -5670,7 +5670,7 @@
       </c>
       <c r="F36" s="22">
         <f>K2*E36</f>
-        <v>24991.738800000003</v>
+        <v>25195.839600000003</v>
       </c>
       <c r="G36" s="22"/>
       <c r="H36" s="10">
@@ -5684,7 +5684,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
       <c r="B37" s="10" t="s">
         <v>86</v>
@@ -5700,7 +5700,7 @@
       </c>
       <c r="F37" s="22">
         <f>K2*E37</f>
-        <v>61836.250000000007</v>
+        <v>62341.25</v>
       </c>
       <c r="G37" s="22"/>
       <c r="H37" s="10">
@@ -5714,7 +5714,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="9"/>
       <c r="B38" s="10" t="s">
         <v>86</v>
@@ -5730,7 +5730,7 @@
       </c>
       <c r="F38" s="22">
         <f>K2*E38</f>
-        <v>24991.738800000003</v>
+        <v>25195.839600000003</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="10">
@@ -5744,7 +5744,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="9"/>
       <c r="B39" s="10" t="s">
         <v>86</v>
@@ -5760,7 +5760,7 @@
       </c>
       <c r="F39" s="22">
         <f>K2*E39</f>
-        <v>24991.738800000003</v>
+        <v>25195.839600000003</v>
       </c>
       <c r="G39" s="22"/>
       <c r="H39" s="10">
@@ -5774,7 +5774,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="9"/>
       <c r="B40" s="10" t="s">
         <v>86</v>
@@ -5790,7 +5790,7 @@
       </c>
       <c r="F40" s="22">
         <f>K2*E40</f>
-        <v>17314.150000000001</v>
+        <v>17455.55</v>
       </c>
       <c r="G40" s="22"/>
       <c r="H40" s="10">
@@ -5804,7 +5804,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
         <v>19</v>
       </c>
@@ -5822,7 +5822,7 @@
       </c>
       <c r="F41" s="22">
         <f>K2*E41</f>
-        <v>22261.050000000003</v>
+        <v>22442.850000000002</v>
       </c>
       <c r="G41" s="22"/>
       <c r="H41" s="10">
@@ -5836,7 +5836,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="9"/>
       <c r="B42" s="10" t="s">
         <v>86</v>
@@ -5852,7 +5852,7 @@
       </c>
       <c r="F42" s="22">
         <f>K2*E42</f>
-        <v>4803.4399000000003</v>
+        <v>4842.6683000000003</v>
       </c>
       <c r="G42" s="22"/>
       <c r="H42" s="10">
@@ -5866,7 +5866,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="9"/>
       <c r="B43" s="10" t="s">
         <v>86</v>
@@ -5882,7 +5882,7 @@
       </c>
       <c r="F43" s="22">
         <f>K2*E43</f>
-        <v>31242.938454000003</v>
+        <v>31498.091118</v>
       </c>
       <c r="G43" s="22"/>
       <c r="H43" s="10">
@@ -5896,7 +5896,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
         <v>19</v>
       </c>
@@ -5914,7 +5914,7 @@
       </c>
       <c r="F44" s="22">
         <f>K2*E44</f>
-        <v>15493.6908</v>
+        <v>15620.223600000001</v>
       </c>
       <c r="G44" s="22"/>
       <c r="H44" s="10">
@@ -5928,7 +5928,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>10</v>
       </c>
@@ -5946,7 +5946,7 @@
       </c>
       <c r="F45" s="22">
         <f>K2*E45</f>
-        <v>31858.036000000004</v>
+        <v>32118.212000000003</v>
       </c>
       <c r="G45" s="22"/>
       <c r="H45" s="10">
@@ -5960,7 +5960,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
         <v>10</v>
       </c>
@@ -5978,7 +5978,7 @@
       </c>
       <c r="F46" s="22">
         <f>K2*E46</f>
-        <v>45832.929561999998</v>
+        <v>46207.234753999997</v>
       </c>
       <c r="G46" s="22"/>
       <c r="H46" s="10">
@@ -5992,7 +5992,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>19</v>
       </c>
@@ -6010,7 +6010,7 @@
       </c>
       <c r="F47" s="22">
         <f>K$2*E47</f>
-        <v>395752</v>
+        <v>398984</v>
       </c>
       <c r="G47" s="22"/>
       <c r="H47" s="10">
@@ -6021,7 +6021,7 @@
       </c>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
         <v>19</v>
       </c>
@@ -6039,7 +6039,7 @@
       </c>
       <c r="F48" s="22">
         <f>K$2*E48</f>
-        <v>262185.7</v>
+        <v>264326.90000000002</v>
       </c>
       <c r="G48" s="22"/>
       <c r="H48" s="10">
@@ -6050,7 +6050,7 @@
       </c>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
         <v>10</v>
       </c>
@@ -6068,7 +6068,7 @@
       </c>
       <c r="F49" s="22">
         <f>K2*E49</f>
-        <v>286722.32400000002</v>
+        <v>289063.908</v>
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="10">
@@ -6082,7 +6082,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
         <v>10</v>
       </c>
@@ -6100,7 +6100,7 @@
       </c>
       <c r="F50" s="22">
         <f>K2*E50</f>
-        <v>24412.951500000003</v>
+        <v>24612.325500000003</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="10">
@@ -6114,7 +6114,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
         <v>10</v>
       </c>
@@ -6132,7 +6132,7 @@
       </c>
       <c r="F51" s="22">
         <f>K2*E51</f>
-        <v>520211.05710000003</v>
+        <v>524459.48070000007</v>
       </c>
       <c r="G51" s="22"/>
       <c r="H51" s="10">
@@ -6146,7 +6146,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="9"/>
       <c r="B52" s="10" t="s">
         <v>132</v>
@@ -6162,7 +6162,7 @@
       </c>
       <c r="F52" s="22">
         <f>K2*E52</f>
-        <v>11130.525000000001</v>
+        <v>11221.425000000001</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="10">
@@ -6176,7 +6176,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="9"/>
       <c r="B53" s="10" t="s">
         <v>132</v>
@@ -6192,7 +6192,7 @@
       </c>
       <c r="F53" s="22">
         <f>K2*E53</f>
-        <v>16596.8495</v>
+        <v>16732.391500000002</v>
       </c>
       <c r="G53" s="22"/>
       <c r="H53" s="10">
@@ -6206,7 +6206,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="9"/>
       <c r="B54" s="10" t="s">
         <v>132</v>
@@ -6222,7 +6222,7 @@
       </c>
       <c r="F54" s="22">
         <f>K2*E54</f>
-        <v>14741.762000000001</v>
+        <v>14862.154</v>
       </c>
       <c r="G54" s="22"/>
       <c r="H54" s="10">
@@ -6236,7 +6236,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="9"/>
       <c r="B55" s="10" t="s">
         <v>137</v>
@@ -6252,7 +6252,7 @@
       </c>
       <c r="F55" s="22">
         <f>K2*E55</f>
-        <v>2707.4878389999999</v>
+        <v>2729.5991629999999</v>
       </c>
       <c r="G55" s="22"/>
       <c r="H55" s="10">
@@ -6266,7 +6266,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="9"/>
       <c r="B56" s="10" t="s">
         <v>137</v>
@@ -6282,7 +6282,7 @@
       </c>
       <c r="F56" s="22">
         <f>K2*E56</f>
-        <v>4729.7805590000007</v>
+        <v>4768.4074030000002</v>
       </c>
       <c r="G56" s="22"/>
       <c r="H56" s="10">
@@ -6296,7 +6296,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="9"/>
       <c r="B57" s="10" t="s">
         <v>137</v>
@@ -6312,7 +6312,7 @@
       </c>
       <c r="F57" s="22">
         <f>K2*E57</f>
-        <v>7420.1026550000006</v>
+        <v>7480.7006350000011</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="10">
@@ -6326,7 +6326,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="9"/>
       <c r="B58" s="10" t="s">
         <v>137</v>
@@ -6342,7 +6342,7 @@
       </c>
       <c r="F58" s="22">
         <f>K2*E58</f>
-        <v>2775.7055900000005</v>
+        <v>2798.3740300000004</v>
       </c>
       <c r="G58" s="22"/>
       <c r="H58" s="10">
@@ -6356,7 +6356,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="9"/>
       <c r="B59" s="10" t="s">
         <v>137</v>
@@ -6372,7 +6372,7 @@
       </c>
       <c r="F59" s="22">
         <f>K2*E59</f>
-        <v>3993.4839630000001</v>
+        <v>4026.097671</v>
       </c>
       <c r="G59" s="22"/>
       <c r="H59" s="10">
@@ -6386,7 +6386,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="9"/>
       <c r="B60" s="10" t="s">
         <v>148</v>
@@ -6402,7 +6402,7 @@
       </c>
       <c r="F60" s="22">
         <f>K2*E60</f>
-        <v>2359.6713</v>
+        <v>2378.9421000000002</v>
       </c>
       <c r="G60" s="22"/>
       <c r="H60" s="10">
@@ -6416,7 +6416,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="9"/>
       <c r="B61" s="10" t="s">
         <v>152</v>
@@ -6432,7 +6432,7 @@
       </c>
       <c r="F61" s="22">
         <f>K2*E61</f>
-        <v>29952.341713000005</v>
+        <v>30196.954421000002</v>
       </c>
       <c r="G61" s="22"/>
       <c r="H61" s="10">
@@ -6446,7 +6446,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="9"/>
       <c r="B62" s="10" t="s">
         <v>152</v>
@@ -6462,7 +6462,7 @@
       </c>
       <c r="F62" s="22">
         <f>K2*E62</f>
-        <v>29952.341713000005</v>
+        <v>30196.954421000002</v>
       </c>
       <c r="G62" s="22"/>
       <c r="H62" s="10">
@@ -6476,7 +6476,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="9"/>
       <c r="B63" s="10" t="s">
         <v>157</v>
@@ -6492,7 +6492,7 @@
       </c>
       <c r="F63" s="22">
         <f>K2*E63</f>
-        <v>97790.319200000013</v>
+        <v>98588.946400000001</v>
       </c>
       <c r="G63" s="22"/>
       <c r="H63" s="10">
@@ -6506,7 +6506,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="9"/>
       <c r="B64" s="10" t="s">
         <v>161</v>
@@ -6522,7 +6522,7 @@
       </c>
       <c r="F64" s="22">
         <f>K2*E64</f>
-        <v>816238.5</v>
+        <v>822904.5</v>
       </c>
       <c r="G64" s="22"/>
       <c r="H64" s="10">
@@ -6536,7 +6536,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="9"/>
       <c r="B65" s="10" t="s">
         <v>164</v>
@@ -6562,7 +6562,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="9"/>
       <c r="B66" s="10" t="s">
         <v>166</v>
@@ -6578,7 +6578,7 @@
       </c>
       <c r="F66" s="22">
         <f>K2*E66</f>
-        <v>42864.888500000001</v>
+        <v>43214.9545</v>
       </c>
       <c r="G66" s="22"/>
       <c r="H66" s="10">
@@ -6592,7 +6592,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="9"/>
       <c r="B67" s="10" t="s">
         <v>166</v>
@@ -6608,7 +6608,7 @@
       </c>
       <c r="F67" s="22">
         <f>K2*E67</f>
-        <v>44225.87962800001</v>
+        <v>44587.060476000006</v>
       </c>
       <c r="G67" s="22"/>
       <c r="H67" s="10">
@@ -6622,7 +6622,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="9"/>
       <c r="B68" s="10" t="s">
         <v>166</v>
@@ -6638,7 +6638,7 @@
       </c>
       <c r="F68" s="22">
         <f>K2*E68</f>
-        <v>44225.87962800001</v>
+        <v>44587.060476000006</v>
       </c>
       <c r="G68" s="22"/>
       <c r="H68" s="10">
@@ -6652,7 +6652,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="9"/>
       <c r="B69" s="10" t="s">
         <v>166</v>
@@ -6668,7 +6668,7 @@
       </c>
       <c r="F69" s="22">
         <f>K2*E69</f>
-        <v>44225.87962800001</v>
+        <v>44587.060476000006</v>
       </c>
       <c r="G69" s="22"/>
       <c r="H69" s="10">
@@ -6682,7 +6682,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="9"/>
       <c r="B70" s="10" t="s">
         <v>166</v>
@@ -6698,7 +6698,7 @@
       </c>
       <c r="F70" s="22">
         <f>K2*E70</f>
-        <v>123969.31400000001</v>
+        <v>124981.73800000001</v>
       </c>
       <c r="G70" s="22"/>
       <c r="H70" s="10">
@@ -6712,7 +6712,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
         <v>19</v>
       </c>
@@ -6730,7 +6730,7 @@
       </c>
       <c r="F71" s="22">
         <f>K2*E71</f>
-        <v>127382.675</v>
+        <v>128422.97500000001</v>
       </c>
       <c r="G71" s="22"/>
       <c r="H71" s="10">
@@ -6744,7 +6744,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="9" t="s">
         <v>19</v>
       </c>
@@ -6762,7 +6762,7 @@
       </c>
       <c r="F72" s="22">
         <f>K2*E72</f>
-        <v>128297.8515</v>
+        <v>129345.62550000001</v>
       </c>
       <c r="G72" s="22"/>
       <c r="H72" s="10">
@@ -6776,7 +6776,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="9" t="s">
         <v>19</v>
       </c>
@@ -6794,7 +6794,7 @@
       </c>
       <c r="F73" s="22">
         <f>K2*E73</f>
-        <v>107842.42000000001</v>
+        <v>108723.14</v>
       </c>
       <c r="G73" s="22"/>
       <c r="H73" s="10">
@@ -6808,7 +6808,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="9" t="s">
         <v>10</v>
       </c>
@@ -6826,7 +6826,7 @@
       </c>
       <c r="F74" s="22">
         <f>K2*E74</f>
-        <v>50977.804500000006</v>
+        <v>51394.126500000006</v>
       </c>
       <c r="G74" s="22"/>
       <c r="H74" s="11">
@@ -6840,7 +6840,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="9" t="s">
         <v>19</v>
       </c>
@@ -6858,7 +6858,7 @@
       </c>
       <c r="F75" s="22">
         <f>K2*E75</f>
-        <v>293252.23200000002</v>
+        <v>295647.14400000003</v>
       </c>
       <c r="G75" s="22"/>
       <c r="H75" s="10">
@@ -6872,7 +6872,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="9"/>
       <c r="B76" s="10" t="s">
         <v>166</v>
@@ -6888,7 +6888,7 @@
       </c>
       <c r="F76" s="22">
         <f>K2*E76</f>
-        <v>107154.8009</v>
+        <v>108029.90530000001</v>
       </c>
       <c r="G76" s="22"/>
       <c r="H76" s="10">
@@ -6902,7 +6902,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="9"/>
       <c r="B77" s="10" t="s">
         <v>184</v>
@@ -6918,7 +6918,7 @@
       </c>
       <c r="F77" s="22">
         <f>K2*E77</f>
-        <v>496.37194600000004</v>
+        <v>500.42568200000005</v>
       </c>
       <c r="G77" s="22"/>
       <c r="H77" s="10">
@@ -6932,7 +6932,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="9"/>
       <c r="B78" s="10" t="s">
         <v>188</v>
@@ -6958,7 +6958,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="9"/>
       <c r="B79" s="10" t="s">
         <v>191</v>
@@ -6974,7 +6974,7 @@
       </c>
       <c r="F79" s="22">
         <f>K2*E79</f>
-        <v>126416.34755400001</v>
+        <v>127448.75581800001</v>
       </c>
       <c r="G79" s="22"/>
       <c r="H79" s="10">
@@ -6988,7 +6988,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="9"/>
       <c r="B80" s="10" t="s">
         <v>195</v>
@@ -7004,7 +7004,7 @@
       </c>
       <c r="F80" s="22">
         <f>K2*E80</f>
-        <v>8273.3439670000007</v>
+        <v>8340.9101390000014</v>
       </c>
       <c r="G80" s="22"/>
       <c r="H80" s="10">
@@ -7018,7 +7018,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="9"/>
       <c r="B81" s="10" t="s">
         <v>199</v>
@@ -7034,7 +7034,7 @@
       </c>
       <c r="F81" s="22">
         <f>K2*E81</f>
-        <v>300771.52</v>
+        <v>303227.84000000003</v>
       </c>
       <c r="G81" s="22"/>
       <c r="H81" s="10">
@@ -7048,7 +7048,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="9"/>
       <c r="B82" s="10" t="s">
         <v>203</v>
@@ -7064,7 +7064,7 @@
       </c>
       <c r="F82" s="22">
         <f>K2*E82</f>
-        <v>41801.305</v>
+        <v>42142.685000000005</v>
       </c>
       <c r="G82" s="22"/>
       <c r="H82" s="10">
@@ -7078,7 +7078,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" s="9"/>
       <c r="B83" s="10" t="s">
         <v>203</v>
@@ -7094,7 +7094,7 @@
       </c>
       <c r="F83" s="22">
         <f>K2*E83</f>
-        <v>41801.305</v>
+        <v>42142.685000000005</v>
       </c>
       <c r="G83" s="22"/>
       <c r="H83" s="10">
@@ -7108,7 +7108,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" s="9"/>
       <c r="B84" s="10" t="s">
         <v>208</v>
@@ -7124,7 +7124,7 @@
       </c>
       <c r="F84" s="22">
         <f>K2*E84</f>
-        <v>1405.3648209999999</v>
+        <v>1416.8420570000001</v>
       </c>
       <c r="G84" s="22"/>
       <c r="H84" s="10">
@@ -7138,7 +7138,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="9"/>
       <c r="B85" s="10" t="s">
         <v>208</v>
@@ -7154,7 +7154,7 @@
       </c>
       <c r="F85" s="22">
         <f>K2*E85</f>
-        <v>1103.1092310000001</v>
+        <v>1112.1180270000002</v>
       </c>
       <c r="G85" s="22"/>
       <c r="H85" s="10">
@@ -7168,7 +7168,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" s="9"/>
       <c r="B86" s="10" t="s">
         <v>212</v>
@@ -7184,7 +7184,7 @@
       </c>
       <c r="F86" s="22">
         <f>K2*E86</f>
-        <v>1282.8795769999999</v>
+        <v>1293.356509</v>
       </c>
       <c r="G86" s="22"/>
       <c r="H86" s="10">
@@ -7198,7 +7198,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="9"/>
       <c r="B87" s="10" t="s">
         <v>214</v>
@@ -7214,7 +7214,7 @@
       </c>
       <c r="F87" s="22">
         <f>K2*E87</f>
-        <v>600.60312899999997</v>
+        <v>605.50809300000003</v>
       </c>
       <c r="G87" s="22"/>
       <c r="H87" s="10">
@@ -7228,7 +7228,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" s="9" t="s">
         <v>19</v>
       </c>
@@ -7246,7 +7246,7 @@
       </c>
       <c r="F88" s="22">
         <f>K2*E88</f>
-        <v>39688.681885999998</v>
+        <v>40012.808662000003</v>
       </c>
       <c r="G88" s="22"/>
       <c r="H88" s="10">
@@ -7260,7 +7260,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" s="9" t="s">
         <v>19</v>
       </c>
@@ -7278,7 +7278,7 @@
       </c>
       <c r="F89" s="22">
         <f>K2*E89</f>
-        <v>39688.681885999998</v>
+        <v>40012.808662000003</v>
       </c>
       <c r="G89" s="22"/>
       <c r="H89" s="10">
@@ -7292,7 +7292,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" s="9" t="s">
         <v>19</v>
       </c>
@@ -7310,7 +7310,7 @@
       </c>
       <c r="F90" s="22">
         <f>K2*E90</f>
-        <v>39688.681885999998</v>
+        <v>40012.808662000003</v>
       </c>
       <c r="G90" s="22"/>
       <c r="H90" s="11">
@@ -7324,7 +7324,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" s="9" t="s">
         <v>19</v>
       </c>
@@ -7342,7 +7342,7 @@
       </c>
       <c r="F91" s="22">
         <f>K2*E91</f>
-        <v>16052.690500000001</v>
+        <v>16183.788500000001</v>
       </c>
       <c r="G91" s="22"/>
       <c r="H91" s="11">
@@ -7356,7 +7356,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" s="9" t="s">
         <v>19</v>
       </c>
@@ -7374,7 +7374,7 @@
       </c>
       <c r="F92" s="22">
         <f>K2*E92</f>
-        <v>16052.690500000001</v>
+        <v>16183.788500000001</v>
       </c>
       <c r="G92" s="22"/>
       <c r="H92" s="10">
@@ -7388,7 +7388,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" s="9"/>
       <c r="B93" s="10" t="s">
         <v>226</v>
@@ -7404,7 +7404,7 @@
       </c>
       <c r="F93" s="22">
         <f>K2*E93</f>
-        <v>69256.600000000006</v>
+        <v>69822.2</v>
       </c>
       <c r="G93" s="22"/>
       <c r="H93" s="10">
@@ -7418,7 +7418,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" s="9"/>
       <c r="B94" s="10" t="s">
         <v>230</v>
@@ -7434,7 +7434,7 @@
       </c>
       <c r="F94" s="22">
         <f>K2*E94</f>
-        <v>8657.0750000000007</v>
+        <v>8727.7749999999996</v>
       </c>
       <c r="G94" s="22"/>
       <c r="H94" s="10">
@@ -7448,7 +7448,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" s="9" t="s">
         <v>19</v>
       </c>
@@ -7466,7 +7466,7 @@
       </c>
       <c r="F95" s="22">
         <f>K2*E95</f>
-        <v>1298163.1729570003</v>
+        <v>1308764.9219690003</v>
       </c>
       <c r="G95" s="22"/>
       <c r="H95" s="10">
@@ -7480,7 +7480,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="9" t="s">
         <v>10</v>
       </c>
@@ -7498,7 +7498,7 @@
       </c>
       <c r="F96" s="22">
         <f>K2*E96</f>
-        <v>24437.686000000002</v>
+        <v>24637.262000000002</v>
       </c>
       <c r="G96" s="22"/>
       <c r="H96" s="10">
@@ -7512,7 +7512,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:13">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" s="9" t="s">
         <v>10</v>
       </c>
@@ -7530,7 +7530,7 @@
       </c>
       <c r="F97" s="22">
         <f>K2*E97</f>
-        <v>64309.700000000004</v>
+        <v>64834.9</v>
       </c>
       <c r="G97" s="22"/>
       <c r="H97" s="10">
@@ -7544,7 +7544,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:13">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" s="9" t="s">
         <v>10</v>
       </c>
@@ -7562,7 +7562,7 @@
       </c>
       <c r="F98" s="22">
         <f>K2*E98</f>
-        <v>64309.700000000004</v>
+        <v>64834.9</v>
       </c>
       <c r="G98" s="22"/>
       <c r="H98" s="10">
@@ -7576,7 +7576,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:13">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" s="9" t="s">
         <v>10</v>
       </c>
@@ -7601,7 +7601,7 @@
       <c r="I99" s="12"/>
       <c r="J99" s="1"/>
     </row>
-    <row r="100" spans="1:13">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" s="9" t="s">
         <v>10</v>
       </c>
@@ -7619,7 +7619,7 @@
       </c>
       <c r="F100" s="22">
         <f>K2*E100</f>
-        <v>24437.686000000002</v>
+        <v>24637.262000000002</v>
       </c>
       <c r="G100" s="22"/>
       <c r="H100" s="10">
@@ -7633,7 +7633,7 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="1:13">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" s="9" t="s">
         <v>19</v>
       </c>
@@ -7651,7 +7651,7 @@
       </c>
       <c r="F101" s="22">
         <f>K2*E101</f>
-        <v>183282.64500000002</v>
+        <v>184779.465</v>
       </c>
       <c r="G101" s="22"/>
       <c r="H101" s="11">
@@ -7665,7 +7665,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="1:13">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102" s="9" t="s">
         <v>19</v>
       </c>
@@ -7683,7 +7683,7 @@
       </c>
       <c r="F102" s="22">
         <f>K2*E102</f>
-        <v>163890.79700000002</v>
+        <v>165229.24900000001</v>
       </c>
       <c r="G102" s="22"/>
       <c r="H102" s="11">
@@ -7697,7 +7697,7 @@
         <v/>
       </c>
     </row>
-    <row r="103" spans="1:13">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" s="9"/>
       <c r="B103" s="10" t="s">
         <v>253</v>
@@ -7713,7 +7713,7 @@
       </c>
       <c r="F103" s="22">
         <f>K2*E103</f>
-        <v>39575.200000000004</v>
+        <v>39898.400000000001</v>
       </c>
       <c r="G103" s="22"/>
       <c r="H103" s="10">
@@ -7727,7 +7727,7 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:13">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104" s="9"/>
       <c r="B104" s="10" t="s">
         <v>257</v>
@@ -7743,7 +7743,7 @@
       </c>
       <c r="F104" s="22">
         <f>K2*E104</f>
-        <v>88302.165000000008</v>
+        <v>89023.305000000008</v>
       </c>
       <c r="G104" s="22"/>
       <c r="H104" s="10">
@@ -7757,7 +7757,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:13">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" s="9" t="s">
         <v>10</v>
       </c>
@@ -7784,7 +7784,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:13">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" s="9" t="s">
         <v>10</v>
       </c>
@@ -7811,7 +7811,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:13">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" s="9" t="s">
         <v>10</v>
       </c>
@@ -7838,7 +7838,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:13" ht="15" thickBot="1">
+    <row r="108" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="9" t="s">
         <v>10</v>
       </c>
@@ -7865,7 +7865,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:13" ht="15" thickBot="1">
+    <row r="109" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="29"/>
       <c r="B109" s="44" t="s">
         <v>265</v>
@@ -7890,7 +7890,7 @@
       <c r="I109" s="26"/>
       <c r="J109" s="1"/>
     </row>
-    <row r="110" spans="1:13" ht="15" thickBot="1">
+    <row r="110" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="29"/>
       <c r="B110" s="41" t="s">
         <v>267</v>
@@ -7913,7 +7913,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="111" spans="1:13" ht="15" thickBot="1">
+    <row r="111" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A111" s="29"/>
       <c r="B111" s="41" t="s">
         <v>269</v>
@@ -7936,7 +7936,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="112" spans="1:13" ht="15" thickBot="1">
+    <row r="112" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="29"/>
       <c r="B112" s="41" t="s">
         <v>270</v>
@@ -7959,7 +7959,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="15" thickBot="1">
+    <row r="113" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="29"/>
       <c r="B113" s="50" t="s">
         <v>271</v>
@@ -7979,7 +7979,7 @@
       <c r="I113" s="26"/>
       <c r="J113" s="1"/>
     </row>
-    <row r="114" spans="1:10" ht="15" thickBot="1">
+    <row r="114" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="29"/>
       <c r="B114" s="50" t="s">
         <v>274</v>
@@ -7999,7 +7999,7 @@
       <c r="I114" s="26"/>
       <c r="J114" s="1"/>
     </row>
-    <row r="115" spans="1:10" ht="15" thickBot="1">
+    <row r="115" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="29"/>
       <c r="B115" s="53" t="s">
         <v>275</v>
@@ -8019,7 +8019,7 @@
       <c r="I115" s="26"/>
       <c r="J115" s="1"/>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" s="9" t="s">
         <v>19</v>
       </c>
@@ -8037,7 +8037,7 @@
       </c>
       <c r="F116" s="22">
         <f>K2*E116</f>
-        <v>54910.590000000004</v>
+        <v>55359.030000000006</v>
       </c>
       <c r="G116" s="22"/>
       <c r="H116" s="43">
@@ -8051,7 +8051,7 @@
         <v/>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" s="9" t="s">
         <v>19</v>
       </c>
@@ -8069,7 +8069,7 @@
       </c>
       <c r="F117" s="22">
         <f>K2*E117</f>
-        <v>70122.30750000001</v>
+        <v>70694.977500000008</v>
       </c>
       <c r="G117" s="22"/>
       <c r="H117" s="11">
@@ -8083,7 +8083,7 @@
         <v/>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" s="9" t="s">
         <v>19</v>
       </c>
@@ -8101,7 +8101,7 @@
       </c>
       <c r="F118" s="22">
         <f>K2*E118</f>
-        <v>17314.150000000001</v>
+        <v>17455.55</v>
       </c>
       <c r="G118" s="22"/>
       <c r="H118" s="10">
@@ -8115,7 +8115,7 @@
         <v/>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" s="9" t="s">
         <v>19</v>
       </c>
@@ -8133,7 +8133,7 @@
       </c>
       <c r="F119" s="22">
         <f>K2*E119</f>
-        <v>17314.150000000001</v>
+        <v>17455.55</v>
       </c>
       <c r="G119" s="22"/>
       <c r="H119" s="11">
@@ -8147,7 +8147,7 @@
         <v/>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" s="9" t="s">
         <v>19</v>
       </c>
@@ -8165,7 +8165,7 @@
       </c>
       <c r="F120" s="22">
         <f>K2*E120</f>
-        <v>31829.739732000002</v>
+        <v>32089.684644000001</v>
       </c>
       <c r="G120" s="22"/>
       <c r="H120" s="10">
@@ -8179,7 +8179,7 @@
         <v/>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" s="9" t="s">
         <v>19</v>
       </c>
@@ -8197,7 +8197,7 @@
       </c>
       <c r="F121" s="22">
         <f>K2*E121</f>
-        <v>28197.33</v>
+        <v>28427.61</v>
       </c>
       <c r="G121" s="22"/>
       <c r="H121" s="10">
@@ -8211,7 +8211,7 @@
         <v/>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" s="9" t="s">
         <v>19</v>
       </c>
@@ -8229,7 +8229,7 @@
       </c>
       <c r="F122" s="22">
         <f>K2*E122</f>
-        <v>3120.0098300000004</v>
+        <v>3145.4901100000002</v>
       </c>
       <c r="G122" s="22"/>
       <c r="H122" s="10">
@@ -8243,7 +8243,7 @@
         <v/>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" s="9" t="s">
         <v>19</v>
       </c>
@@ -8261,7 +8261,7 @@
       </c>
       <c r="F123" s="22">
         <f>K$2*E123</f>
-        <v>89928.458375000002</v>
+        <v>90662.879874999999</v>
       </c>
       <c r="G123" s="22"/>
       <c r="H123" s="10">
@@ -8272,7 +8272,7 @@
       </c>
       <c r="J123" s="1"/>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124" s="9" t="s">
         <v>19</v>
       </c>
@@ -8290,7 +8290,7 @@
       </c>
       <c r="F124" s="22">
         <f>K$2*E124</f>
-        <v>74203.5</v>
+        <v>74809.5</v>
       </c>
       <c r="G124" s="22"/>
       <c r="H124" s="10">
@@ -8301,7 +8301,7 @@
       </c>
       <c r="J124" s="1"/>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125" s="9"/>
       <c r="B125" s="10" t="s">
         <v>301</v>
@@ -8317,7 +8317,7 @@
       </c>
       <c r="F125" s="22">
         <f>K2*E125</f>
-        <v>5580.3010759999997</v>
+        <v>5625.8738920000005</v>
       </c>
       <c r="G125" s="22"/>
       <c r="H125" s="10">
@@ -8331,7 +8331,7 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A126" s="9"/>
       <c r="B126" s="10" t="s">
         <v>305</v>
@@ -8347,7 +8347,7 @@
       </c>
       <c r="F126" s="22">
         <f>K2*E126</f>
-        <v>330823.9375</v>
+        <v>333525.6875</v>
       </c>
       <c r="G126" s="22"/>
       <c r="H126" s="10">
@@ -8361,7 +8361,7 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127" s="9"/>
       <c r="B127" s="10" t="s">
         <v>308</v>
@@ -8377,7 +8377,7 @@
       </c>
       <c r="F127" s="22">
         <f>K2*E127</f>
-        <v>470774.01407400006</v>
+        <v>474618.69865800004</v>
       </c>
       <c r="G127" s="22"/>
       <c r="H127" s="10">
@@ -8391,7 +8391,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A128" s="9"/>
       <c r="B128" s="10" t="s">
         <v>311</v>
@@ -8417,7 +8417,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:13">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129" s="9" t="s">
         <v>19</v>
       </c>
@@ -8435,7 +8435,7 @@
       </c>
       <c r="F129" s="22">
         <f>K2*E129</f>
-        <v>34380.955000000002</v>
+        <v>34661.735000000001</v>
       </c>
       <c r="G129" s="22"/>
       <c r="H129" s="10">
@@ -8452,7 +8452,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="130" spans="1:13">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130" s="9"/>
       <c r="B130" s="10" t="s">
         <v>313</v>
@@ -8468,7 +8468,7 @@
       </c>
       <c r="F130" s="22">
         <f>K2*E130</f>
-        <v>42716.481500000002</v>
+        <v>43065.335500000001</v>
       </c>
       <c r="G130" s="22"/>
       <c r="H130" s="10">
@@ -8485,7 +8485,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="131" spans="1:13">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131" s="9"/>
       <c r="B131" s="10" t="s">
         <v>319</v>
@@ -8508,7 +8508,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="132" spans="1:13">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A132" s="9"/>
       <c r="B132" s="10" t="s">
         <v>320</v>
@@ -8524,7 +8524,7 @@
       </c>
       <c r="F132" s="22">
         <f>K2*E132</f>
-        <v>4793.5461000000005</v>
+        <v>4832.6937000000007</v>
       </c>
       <c r="G132" s="22"/>
       <c r="H132" s="10">
@@ -8538,7 +8538,7 @@
         <v/>
       </c>
     </row>
-    <row r="133" spans="1:13">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133" s="9"/>
       <c r="B133" s="10" t="s">
         <v>320</v>
@@ -8565,7 +8565,7 @@
         <v/>
       </c>
     </row>
-    <row r="134" spans="1:13">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134" s="9"/>
       <c r="B134" s="10" t="s">
         <v>320</v>
@@ -8581,7 +8581,7 @@
       </c>
       <c r="F134" s="22">
         <f>K2*E134</f>
-        <v>16210.991300000002</v>
+        <v>16343.382100000001</v>
       </c>
       <c r="G134" s="22"/>
       <c r="H134" s="10">
@@ -8595,7 +8595,7 @@
         <v/>
       </c>
     </row>
-    <row r="135" spans="1:13" ht="15" thickBot="1">
+    <row r="135" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A135" s="9" t="s">
         <v>19</v>
       </c>
@@ -8613,7 +8613,7 @@
       </c>
       <c r="F135" s="22">
         <f>K2*E135</f>
-        <v>38875.460995000001</v>
+        <v>39192.946415000006</v>
       </c>
       <c r="G135" s="22"/>
       <c r="H135" s="16">
@@ -8627,7 +8627,7 @@
         <v/>
       </c>
     </row>
-    <row r="136" spans="1:13" ht="15" thickBot="1">
+    <row r="136" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A136" s="29"/>
       <c r="B136" s="59" t="s">
         <v>330</v>
@@ -8647,7 +8647,7 @@
       <c r="I136" s="26"/>
       <c r="J136" s="1"/>
     </row>
-    <row r="137" spans="1:13" ht="15" thickBot="1">
+    <row r="137" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A137" s="29"/>
       <c r="B137" s="62" t="s">
         <v>332</v>
@@ -8667,7 +8667,7 @@
       <c r="I137" s="26"/>
       <c r="J137" s="1"/>
     </row>
-    <row r="138" spans="1:13" ht="15" thickBot="1">
+    <row r="138" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A138" s="29"/>
       <c r="B138" s="62" t="s">
         <v>333</v>
@@ -8687,7 +8687,7 @@
       <c r="I138" s="26"/>
       <c r="J138" s="1"/>
     </row>
-    <row r="139" spans="1:13" ht="15" thickBot="1">
+    <row r="139" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A139" s="29"/>
       <c r="B139" s="65" t="s">
         <v>334</v>
@@ -8707,7 +8707,7 @@
       <c r="I139" s="26"/>
       <c r="J139" s="1"/>
     </row>
-    <row r="140" spans="1:13" ht="15" thickBot="1">
+    <row r="140" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="29"/>
       <c r="B140" s="68" t="s">
         <v>335</v>
@@ -8723,7 +8723,7 @@
       </c>
       <c r="F140" s="22">
         <f>K2*E140</f>
-        <v>1810565.4000000001</v>
+        <v>1825351.8</v>
       </c>
       <c r="G140" s="22"/>
       <c r="H140" s="79">
@@ -8740,7 +8740,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="141" spans="1:13" ht="15" thickBot="1">
+    <row r="141" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="29"/>
       <c r="B141" s="68" t="s">
         <v>338</v>
@@ -8763,7 +8763,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="142" spans="1:13" ht="15" thickBot="1">
+    <row r="142" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A142" s="29"/>
       <c r="B142" s="68" t="s">
         <v>339</v>
@@ -8786,7 +8786,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="143" spans="1:13" ht="15" thickBot="1">
+    <row r="143" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="29"/>
       <c r="B143" s="68" t="s">
         <v>340</v>
@@ -8809,7 +8809,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="144" spans="1:13" ht="15" thickBot="1">
+    <row r="144" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A144" s="29" t="s">
         <v>10</v>
       </c>
@@ -8827,7 +8827,7 @@
       </c>
       <c r="F144" s="22">
         <f>K2*E144</f>
-        <v>1810565.4000000001</v>
+        <v>1825351.8</v>
       </c>
       <c r="G144" s="22"/>
       <c r="H144" s="79">
@@ -8844,7 +8844,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="145" spans="1:13" ht="15" thickBot="1">
+    <row r="145" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="29"/>
       <c r="B145" s="71" t="s">
         <v>344</v>
@@ -8867,7 +8867,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="146" spans="1:13" ht="15" thickBot="1">
+    <row r="146" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="29"/>
       <c r="B146" s="68" t="s">
         <v>345</v>
@@ -8890,7 +8890,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="147" spans="1:13" ht="15" thickBot="1">
+    <row r="147" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A147" s="29"/>
       <c r="B147" s="74" t="s">
         <v>346</v>
@@ -8913,7 +8913,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="148" spans="1:13">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A148" s="9"/>
       <c r="B148" s="28" t="s">
         <v>347</v>
@@ -8929,7 +8929,7 @@
       </c>
       <c r="F148" s="22">
         <f>K2*E148</f>
-        <v>3784.0322169999999</v>
+        <v>3814.9353889999998</v>
       </c>
       <c r="G148" s="22"/>
       <c r="H148" s="28">
@@ -8943,7 +8943,7 @@
         <v/>
       </c>
     </row>
-    <row r="149" spans="1:13">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A149" s="9"/>
       <c r="B149" s="10" t="s">
         <v>351</v>
@@ -8959,7 +8959,7 @@
       </c>
       <c r="F149" s="22">
         <f>K2*E149</f>
-        <v>231.119168</v>
+        <v>233.00665600000002</v>
       </c>
       <c r="G149" s="22"/>
       <c r="H149" s="10">
@@ -8973,7 +8973,7 @@
         <v/>
       </c>
     </row>
-    <row r="150" spans="1:13">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A150" s="9"/>
       <c r="B150" s="10" t="s">
         <v>355</v>
@@ -8989,7 +8989,7 @@
       </c>
       <c r="F150" s="22">
         <f>K2*E150</f>
-        <v>124196.32724100001</v>
+        <v>125210.605197</v>
       </c>
       <c r="G150" s="22"/>
       <c r="H150" s="10">
@@ -9003,7 +9003,7 @@
         <v/>
       </c>
     </row>
-    <row r="151" spans="1:13">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A151" s="9"/>
       <c r="B151" s="10" t="s">
         <v>358</v>
@@ -9019,7 +9019,7 @@
       </c>
       <c r="F151" s="22">
         <f>K2*E151</f>
-        <v>2611.9632000000001</v>
+        <v>2633.2944000000002</v>
       </c>
       <c r="G151" s="22"/>
       <c r="H151" s="10">
@@ -9033,7 +9033,7 @@
         <v/>
       </c>
     </row>
-    <row r="152" spans="1:13">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A152" s="9"/>
       <c r="B152" s="10" t="s">
         <v>362</v>
@@ -9049,7 +9049,7 @@
       </c>
       <c r="F152" s="22">
         <f>K2*E152</f>
-        <v>113006.98360000001</v>
+        <v>113929.8812</v>
       </c>
       <c r="G152" s="22"/>
       <c r="H152" s="10">
@@ -9063,7 +9063,7 @@
         <v/>
       </c>
     </row>
-    <row r="153" spans="1:13" ht="16.899999999999999" customHeight="1" thickBot="1">
+    <row r="153" spans="1:13" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A153" s="15"/>
       <c r="B153" s="16" t="s">
         <v>362</v>
@@ -9079,7 +9079,7 @@
       </c>
       <c r="F153" s="22">
         <f>K2*E153</f>
-        <v>132004.06898000001</v>
+        <v>133082.11066000001</v>
       </c>
       <c r="G153" s="22"/>
       <c r="H153" s="16">
@@ -9093,7 +9093,7 @@
         <v/>
       </c>
     </row>
-    <row r="154" spans="1:13" ht="15" thickBot="1">
+    <row r="154" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A154" s="30" t="s">
         <v>19</v>
       </c>
@@ -9111,7 +9111,7 @@
       </c>
       <c r="F154" s="22">
         <f>K2*E154</f>
-        <v>1488358.9623</v>
+        <v>1500513.9891000001</v>
       </c>
       <c r="G154" s="22"/>
       <c r="H154" s="99">
@@ -9128,7 +9128,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="155" spans="1:13" ht="15" thickBot="1">
+    <row r="155" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A155" s="31"/>
       <c r="B155" s="79" t="s">
         <v>368</v>
@@ -9151,7 +9151,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="156" spans="1:13" ht="15" thickBot="1">
+    <row r="156" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A156" s="31"/>
       <c r="B156" s="80" t="s">
         <v>369</v>
@@ -9174,7 +9174,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="157" spans="1:13" ht="15" thickBot="1">
+    <row r="157" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A157" s="31"/>
       <c r="B157" s="80" t="s">
         <v>370</v>
@@ -9197,7 +9197,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="158" spans="1:13" ht="15" thickBot="1">
+    <row r="158" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A158" s="31"/>
       <c r="B158" s="80" t="s">
         <v>371</v>
@@ -9220,7 +9220,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="159" spans="1:13" ht="15" thickBot="1">
+    <row r="159" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A159" s="32"/>
       <c r="B159" s="83" t="s">
         <v>372</v>
@@ -9243,7 +9243,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="160" spans="1:13">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A160" s="27"/>
       <c r="B160" s="28" t="s">
         <v>373</v>
@@ -9259,7 +9259,7 @@
       </c>
       <c r="F160" s="22">
         <f>K2*E160</f>
-        <v>399025.36372999998</v>
+        <v>402284.09641</v>
       </c>
       <c r="G160" s="22"/>
       <c r="H160" s="28">
@@ -9273,7 +9273,7 @@
         <v/>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A161" s="9"/>
       <c r="B161" s="10" t="s">
         <v>377</v>
@@ -9289,7 +9289,7 @@
       </c>
       <c r="F161" s="22">
         <f>K2*E161</f>
-        <v>9092.4022000000004</v>
+        <v>9166.6574000000001</v>
       </c>
       <c r="G161" s="22"/>
       <c r="H161" s="10">
@@ -9303,7 +9303,7 @@
         <v/>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A162" s="9"/>
       <c r="B162" s="10" t="s">
         <v>381</v>
@@ -9319,7 +9319,7 @@
       </c>
       <c r="F162" s="22">
         <f>K2*E162</f>
-        <v>25995.959500000001</v>
+        <v>26208.261500000001</v>
       </c>
       <c r="G162" s="22"/>
       <c r="H162" s="10">
@@ -9333,7 +9333,7 @@
         <v/>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A163" s="9"/>
       <c r="B163" s="10" t="s">
         <v>383</v>
@@ -9349,7 +9349,7 @@
       </c>
       <c r="F163" s="22">
         <f>K2*E163</f>
-        <v>816.23850000000004</v>
+        <v>822.9045000000001</v>
       </c>
       <c r="G163" s="22"/>
       <c r="H163" s="10">
@@ -9363,7 +9363,7 @@
         <v/>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A164" s="9"/>
       <c r="B164" s="10" t="s">
         <v>387</v>
@@ -9389,7 +9389,7 @@
         <v/>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A165" s="9"/>
       <c r="B165" s="10" t="s">
         <v>390</v>
@@ -9405,7 +9405,7 @@
       </c>
       <c r="F165" s="22">
         <f>K2*E165</f>
-        <v>2621.857</v>
+        <v>2643.2690000000002</v>
       </c>
       <c r="G165" s="22"/>
       <c r="H165" s="10">
@@ -9419,7 +9419,7 @@
         <v/>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A166" s="9"/>
       <c r="B166" s="10" t="s">
         <v>392</v>
@@ -9435,7 +9435,7 @@
       </c>
       <c r="F166" s="22">
         <f>K2*E166</f>
-        <v>203812.28</v>
+        <v>205476.76</v>
       </c>
       <c r="G166" s="22"/>
       <c r="H166" s="10">
@@ -9449,7 +9449,7 @@
         <v/>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A167" s="9" t="s">
         <v>10</v>
       </c>
@@ -9467,7 +9467,7 @@
       </c>
       <c r="F167" s="22">
         <f t="shared" ref="F167:F168" si="0">K$2*E167</f>
-        <v>415539.60000000003</v>
+        <v>418933.2</v>
       </c>
       <c r="G167" s="22"/>
       <c r="H167" s="10">
@@ -9476,7 +9476,7 @@
       <c r="I167" s="12"/>
       <c r="J167" s="1"/>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A168" s="9" t="s">
         <v>10</v>
       </c>
@@ -9494,7 +9494,7 @@
       </c>
       <c r="F168" s="22">
         <f t="shared" si="0"/>
-        <v>415539.60000000003</v>
+        <v>418933.2</v>
       </c>
       <c r="G168" s="22"/>
       <c r="H168" s="10">
@@ -9503,7 +9503,7 @@
       <c r="I168" s="12"/>
       <c r="J168" s="1"/>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A169" s="9" t="s">
         <v>10</v>
       </c>
@@ -9521,7 +9521,7 @@
       </c>
       <c r="F169" s="22">
         <f>K$2*E169</f>
-        <v>415539.60000000003</v>
+        <v>418933.2</v>
       </c>
       <c r="G169" s="22"/>
       <c r="H169" s="10">
@@ -9535,7 +9535,7 @@
         <v/>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A170" s="9"/>
       <c r="B170" s="10" t="s">
         <v>404</v>
@@ -9551,7 +9551,7 @@
       </c>
       <c r="F170" s="22">
         <f>K2*E170</f>
-        <v>12317.781000000001</v>
+        <v>12418.377</v>
       </c>
       <c r="G170" s="22"/>
       <c r="H170" s="10">
@@ -9565,7 +9565,7 @@
         <v/>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A171" s="9" t="s">
         <v>10</v>
       </c>
@@ -9583,7 +9583,7 @@
       </c>
       <c r="F171" s="22">
         <f>K2*E171</f>
-        <v>273266.75599999999</v>
+        <v>275498.45199999999</v>
       </c>
       <c r="G171" s="22"/>
       <c r="H171" s="11">
@@ -9597,7 +9597,7 @@
         <v/>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A172" s="9"/>
       <c r="B172" s="10" t="s">
         <v>411</v>
@@ -9613,7 +9613,7 @@
       </c>
       <c r="F172" s="22">
         <f>K2*E172</f>
-        <v>63097.709500000004</v>
+        <v>63613.011500000001</v>
       </c>
       <c r="G172" s="22"/>
       <c r="H172" s="10">
@@ -9627,7 +9627,7 @@
         <v/>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A173" s="9" t="s">
         <v>19</v>
       </c>
@@ -9645,7 +9645,7 @@
       </c>
       <c r="F173" s="22">
         <f>K2*E173</f>
-        <v>28345.737000000001</v>
+        <v>28577.229000000003</v>
       </c>
       <c r="G173" s="22"/>
       <c r="H173" s="11">
@@ -9659,7 +9659,7 @@
         <v/>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A174" s="9" t="s">
         <v>19</v>
       </c>
@@ -9677,7 +9677,7 @@
       </c>
       <c r="F174" s="22">
         <f>K2*E174</f>
-        <v>37126.484499999999</v>
+        <v>37429.686500000003</v>
       </c>
       <c r="G174" s="22"/>
       <c r="H174" s="10">
@@ -9689,7 +9689,7 @@
         <v/>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A175" s="9" t="s">
         <v>19</v>
       </c>
@@ -9707,7 +9707,7 @@
       </c>
       <c r="F175" s="22">
         <f>K2*E175</f>
-        <v>20282.29</v>
+        <v>20447.93</v>
       </c>
       <c r="G175" s="22"/>
       <c r="H175" s="10">
@@ -9721,7 +9721,7 @@
         <v/>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A176" s="9" t="s">
         <v>19</v>
       </c>
@@ -9739,7 +9739,7 @@
       </c>
       <c r="F176" s="22">
         <f>K2*E176</f>
-        <v>30101.886500000001</v>
+        <v>30347.720500000003</v>
       </c>
       <c r="G176" s="22"/>
       <c r="H176" s="10">
@@ -9753,7 +9753,7 @@
         <v/>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A177" s="9" t="s">
         <v>19</v>
       </c>
@@ -9771,7 +9771,7 @@
       </c>
       <c r="F177" s="22">
         <f>K2*E177</f>
-        <v>31091.266500000002</v>
+        <v>31345.180500000002</v>
       </c>
       <c r="G177" s="22"/>
       <c r="H177" s="10">
@@ -9785,7 +9785,7 @@
         <v/>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A178" s="9"/>
       <c r="B178" s="10" t="s">
         <v>425</v>
@@ -9801,7 +9801,7 @@
       </c>
       <c r="F178" s="22">
         <f>K2*E178</f>
-        <v>8854.9510000000009</v>
+        <v>8927.2669999999998</v>
       </c>
       <c r="G178" s="22"/>
       <c r="H178" s="10">
@@ -9815,7 +9815,7 @@
         <v/>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A179" s="9"/>
       <c r="B179" s="10" t="s">
         <v>427</v>
@@ -9831,7 +9831,7 @@
       </c>
       <c r="F179" s="22">
         <f>K2*E179</f>
-        <v>20133.883000000002</v>
+        <v>20298.311000000002</v>
       </c>
       <c r="G179" s="22"/>
       <c r="H179" s="10">
@@ -9845,7 +9845,7 @@
         <v/>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A180" s="9"/>
       <c r="B180" s="10" t="s">
         <v>430</v>
@@ -9871,7 +9871,7 @@
         <v/>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A181" s="9" t="s">
         <v>19</v>
       </c>
@@ -9889,7 +9889,7 @@
       </c>
       <c r="F181" s="22">
         <f>K2*E181</f>
-        <v>26465.915000000001</v>
+        <v>26682.055</v>
       </c>
       <c r="G181" s="22"/>
       <c r="H181" s="11">
@@ -9903,7 +9903,7 @@
         <v/>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A182" s="9" t="s">
         <v>19</v>
       </c>
@@ -9921,7 +9921,7 @@
       </c>
       <c r="F182" s="22">
         <f>K2*E182</f>
-        <v>12660.897984000001</v>
+        <v>12764.296128000002</v>
       </c>
       <c r="G182" s="22"/>
       <c r="H182" s="11">
@@ -9935,7 +9935,7 @@
         <v/>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A183" s="9"/>
       <c r="B183" s="10" t="s">
         <v>437</v>
@@ -9951,7 +9951,7 @@
       </c>
       <c r="F183" s="22">
         <f>K2*E183</f>
-        <v>1681.9460000000001</v>
+        <v>1695.682</v>
       </c>
       <c r="G183" s="22"/>
       <c r="H183" s="10">
@@ -9965,7 +9965,7 @@
         <v/>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A184" s="9"/>
       <c r="B184" s="10" t="s">
         <v>441</v>
@@ -9981,7 +9981,7 @@
       </c>
       <c r="F184" s="22">
         <f>K2*E184</f>
-        <v>13831.730276</v>
+        <v>13944.690292000001</v>
       </c>
       <c r="G184" s="22"/>
       <c r="H184" s="10">
@@ -9995,7 +9995,7 @@
         <v/>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A185" s="9" t="s">
         <v>19</v>
       </c>
@@ -10013,7 +10013,7 @@
       </c>
       <c r="F185" s="22">
         <f>K2*E185</f>
-        <v>18080.9195</v>
+        <v>18228.5815</v>
       </c>
       <c r="G185" s="22"/>
       <c r="H185" s="10">
@@ -10027,7 +10027,7 @@
         <v/>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A186" s="9" t="s">
         <v>19</v>
       </c>
@@ -10045,7 +10045,7 @@
       </c>
       <c r="F186" s="22">
         <f>K2*E186</f>
-        <v>22279.254592000001</v>
+        <v>22461.203264000003</v>
       </c>
       <c r="G186" s="22"/>
       <c r="H186" s="10">
@@ -10059,7 +10059,7 @@
         <v/>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A187" s="9" t="s">
         <v>19</v>
       </c>
@@ -10077,7 +10077,7 @@
       </c>
       <c r="F187" s="22">
         <f>K2*E187</f>
-        <v>4031.7235000000001</v>
+        <v>4064.6495000000004</v>
       </c>
       <c r="G187" s="22"/>
       <c r="H187" s="10">
@@ -10091,7 +10091,7 @@
         <v/>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A188" s="9"/>
       <c r="B188" s="10" t="s">
         <v>447</v>
@@ -10107,7 +10107,7 @@
       </c>
       <c r="F188" s="22">
         <f>K2*E188</f>
-        <v>14797.266218000001</v>
+        <v>14918.111505999999</v>
       </c>
       <c r="G188" s="22"/>
       <c r="H188" s="10">
@@ -10121,7 +10121,7 @@
         <v/>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A189" s="9"/>
       <c r="B189" s="10" t="s">
         <v>451</v>
@@ -10137,7 +10137,7 @@
       </c>
       <c r="F189" s="22">
         <f>K2*E189</f>
-        <v>11971.498000000001</v>
+        <v>12069.266000000001</v>
       </c>
       <c r="G189" s="22"/>
       <c r="H189" s="10">
@@ -10151,7 +10151,7 @@
         <v/>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A190" s="9"/>
       <c r="B190" s="10" t="s">
         <v>451</v>
@@ -10167,7 +10167,7 @@
       </c>
       <c r="F190" s="22">
         <f>K2*E190</f>
-        <v>18451.937000000002</v>
+        <v>18602.629000000001</v>
       </c>
       <c r="G190" s="22"/>
       <c r="H190" s="10">
@@ -10181,7 +10181,7 @@
         <v/>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A191" s="9"/>
       <c r="B191" s="10" t="s">
         <v>451</v>
@@ -10197,7 +10197,7 @@
       </c>
       <c r="F191" s="22">
         <f>K2*E191</f>
-        <v>36557.591</v>
+        <v>36856.147000000004</v>
       </c>
       <c r="G191" s="22"/>
       <c r="H191" s="10">
@@ -10211,7 +10211,7 @@
         <v/>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A192" s="9"/>
       <c r="B192" s="86" t="s">
         <v>455</v>
@@ -10241,7 +10241,7 @@
         <v/>
       </c>
     </row>
-    <row r="193" spans="1:16 16378:16382">
+    <row r="193" spans="1:16 16378:16382" x14ac:dyDescent="0.3">
       <c r="A193" s="9"/>
       <c r="B193" s="10" t="s">
         <v>459</v>
@@ -10267,7 +10267,7 @@
         <v/>
       </c>
     </row>
-    <row r="194" spans="1:16 16378:16382">
+    <row r="194" spans="1:16 16378:16382" x14ac:dyDescent="0.3">
       <c r="A194" s="9"/>
       <c r="B194" s="10" t="s">
         <v>461</v>
@@ -10283,7 +10283,7 @@
       </c>
       <c r="F194" s="22">
         <f>K2*E194</f>
-        <v>37126.484499999999</v>
+        <v>37429.686500000003</v>
       </c>
       <c r="G194" s="22"/>
       <c r="H194" s="10">
@@ -10297,7 +10297,7 @@
         <v/>
       </c>
     </row>
-    <row r="195" spans="1:16 16378:16382">
+    <row r="195" spans="1:16 16378:16382" x14ac:dyDescent="0.3">
       <c r="A195" s="9"/>
       <c r="B195" s="10" t="s">
         <v>464</v>
@@ -10313,7 +10313,7 @@
       </c>
       <c r="F195" s="22">
         <f>K2*E195</f>
-        <v>47119.222500000003</v>
+        <v>47504.032500000001</v>
       </c>
       <c r="G195" s="22"/>
       <c r="H195" s="10">
@@ -10327,7 +10327,7 @@
         <v/>
       </c>
     </row>
-    <row r="196" spans="1:16 16378:16382" ht="15" thickBot="1">
+    <row r="196" spans="1:16 16378:16382" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A196" s="9" t="s">
         <v>10</v>
       </c>
@@ -10345,7 +10345,7 @@
       </c>
       <c r="F196" s="22">
         <f>K2*E196</f>
-        <v>194917.75380000001</v>
+        <v>196509.59460000001</v>
       </c>
       <c r="G196" s="22"/>
       <c r="H196" s="10">
@@ -10359,7 +10359,7 @@
         <v/>
       </c>
     </row>
-    <row r="197" spans="1:16 16378:16382" ht="15" thickBot="1">
+    <row r="197" spans="1:16 16378:16382" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A197" s="29" t="s">
         <v>10</v>
       </c>
@@ -10377,7 +10377,7 @@
       </c>
       <c r="F197" s="22">
         <f>K2*E197</f>
-        <v>238687.92500000002</v>
+        <v>240637.22500000001</v>
       </c>
       <c r="G197" s="22"/>
       <c r="H197" s="79">
@@ -10391,7 +10391,7 @@
         <v/>
       </c>
     </row>
-    <row r="198" spans="1:16 16378:16382" ht="15" thickBot="1">
+    <row r="198" spans="1:16 16378:16382" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A198" s="29"/>
       <c r="B198" s="89" t="s">
         <v>469</v>
@@ -10411,7 +10411,7 @@
       <c r="I198" s="26"/>
       <c r="J198" s="1"/>
     </row>
-    <row r="199" spans="1:16 16378:16382" ht="15" thickBot="1">
+    <row r="199" spans="1:16 16378:16382" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A199" s="29"/>
       <c r="B199" s="71" t="s">
         <v>470</v>
@@ -10431,7 +10431,7 @@
       <c r="I199" s="26"/>
       <c r="J199" s="1"/>
     </row>
-    <row r="200" spans="1:16 16378:16382" ht="15" thickBot="1">
+    <row r="200" spans="1:16 16378:16382" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A200" s="29"/>
       <c r="B200" s="94" t="s">
         <v>472</v>
@@ -10454,7 +10454,7 @@
       <c r="XFA200" s="38"/>
       <c r="XFB200" s="39"/>
     </row>
-    <row r="201" spans="1:16 16378:16382" ht="15" thickBot="1">
+    <row r="201" spans="1:16 16378:16382" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A201" s="9" t="s">
         <v>10</v>
       </c>
@@ -10472,7 +10472,7 @@
       </c>
       <c r="F201" s="22">
         <f>K2*E201</f>
-        <v>151152.5295</v>
+        <v>152386.9515</v>
       </c>
       <c r="G201" s="22"/>
       <c r="H201" s="69">
@@ -10486,7 +10486,7 @@
         <v/>
       </c>
     </row>
-    <row r="202" spans="1:16 16378:16382" ht="15" thickBot="1">
+    <row r="202" spans="1:16 16378:16382" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A202" s="9"/>
       <c r="B202" s="69" t="s">
         <v>472</v>
@@ -10506,7 +10506,7 @@
       <c r="I202" s="12"/>
       <c r="J202" s="1"/>
     </row>
-    <row r="203" spans="1:16 16378:16382" ht="15" thickBot="1">
+    <row r="203" spans="1:16 16378:16382" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A203" s="29"/>
       <c r="B203" s="68" t="s">
         <v>475</v>
@@ -10526,7 +10526,7 @@
       <c r="I203" s="26"/>
       <c r="J203" s="1"/>
     </row>
-    <row r="204" spans="1:16 16378:16382" ht="15" thickBot="1">
+    <row r="204" spans="1:16 16378:16382" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A204" s="29"/>
       <c r="B204" s="68" t="s">
         <v>476</v>
@@ -10546,7 +10546,7 @@
       <c r="I204" s="26"/>
       <c r="J204" s="1"/>
     </row>
-    <row r="205" spans="1:16 16378:16382">
+    <row r="205" spans="1:16 16378:16382" x14ac:dyDescent="0.3">
       <c r="A205" s="9"/>
       <c r="B205" s="28" t="s">
         <v>477</v>
@@ -10562,7 +10562,7 @@
       </c>
       <c r="F205" s="22">
         <f>K2*E205</f>
-        <v>3759.6440000000002</v>
+        <v>3790.3480000000004</v>
       </c>
       <c r="G205" s="22"/>
       <c r="H205" s="28">
@@ -10576,7 +10576,7 @@
         <v/>
       </c>
     </row>
-    <row r="206" spans="1:16 16378:16382">
+    <row r="206" spans="1:16 16378:16382" x14ac:dyDescent="0.3">
       <c r="A206" s="9"/>
       <c r="B206" s="10" t="s">
         <v>481</v>
@@ -10592,7 +10592,7 @@
       </c>
       <c r="F206" s="22">
         <f>K2*E206</f>
-        <v>6307.2975000000006</v>
+        <v>6358.8075000000008</v>
       </c>
       <c r="G206" s="22"/>
       <c r="H206" s="10">
@@ -10606,7 +10606,7 @@
         <v/>
       </c>
     </row>
-    <row r="207" spans="1:16 16378:16382">
+    <row r="207" spans="1:16 16378:16382" x14ac:dyDescent="0.3">
       <c r="A207" s="9"/>
       <c r="B207" s="10" t="s">
         <v>485</v>
@@ -10632,7 +10632,7 @@
         <v/>
       </c>
     </row>
-    <row r="208" spans="1:16 16378:16382">
+    <row r="208" spans="1:16 16378:16382" x14ac:dyDescent="0.3">
       <c r="A208" s="9"/>
       <c r="B208" s="10" t="s">
         <v>487</v>
@@ -10648,7 +10648,7 @@
       </c>
       <c r="F208" s="22">
         <f>K2*E208</f>
-        <v>32154.850000000002</v>
+        <v>32417.45</v>
       </c>
       <c r="G208" s="22"/>
       <c r="H208" s="10">
@@ -10663,7 +10663,7 @@
       </c>
       <c r="P208" s="58"/>
     </row>
-    <row r="209" spans="1:10" ht="15" thickBot="1">
+    <row r="209" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A209" s="9" t="s">
         <v>10</v>
       </c>
@@ -10681,7 +10681,7 @@
       </c>
       <c r="F209" s="22">
         <f>K2*E209</f>
-        <v>400698.9</v>
+        <v>403971.30000000005</v>
       </c>
       <c r="G209" s="22"/>
       <c r="H209" s="16">
@@ -10695,7 +10695,7 @@
         <v/>
       </c>
     </row>
-    <row r="210" spans="1:10" ht="15" thickBot="1">
+    <row r="210" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A210" s="29" t="s">
         <v>10</v>
       </c>
@@ -10713,7 +10713,7 @@
       </c>
       <c r="F210" s="22">
         <f>K2*E210</f>
-        <v>348066.75320200005</v>
+        <v>350909.320634</v>
       </c>
       <c r="G210" s="22"/>
       <c r="H210" s="89">
@@ -10727,7 +10727,7 @@
         <v/>
       </c>
     </row>
-    <row r="211" spans="1:10" ht="15" thickBot="1">
+    <row r="211" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A211" s="29"/>
       <c r="B211" s="79" t="s">
         <v>496</v>
@@ -10747,7 +10747,7 @@
       <c r="I211" s="26"/>
       <c r="J211" s="1"/>
     </row>
-    <row r="212" spans="1:10" ht="15" thickBot="1">
+    <row r="212" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A212" s="29"/>
       <c r="B212" s="95" t="s">
         <v>497</v>
@@ -10767,7 +10767,7 @@
       <c r="I212" s="26"/>
       <c r="J212" s="1"/>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A213" s="9" t="s">
         <v>10</v>
       </c>
@@ -10785,7 +10785,7 @@
       </c>
       <c r="F213" s="22">
         <f>K2*E213</f>
-        <v>335577.90840000001</v>
+        <v>338318.4828</v>
       </c>
       <c r="G213" s="22"/>
       <c r="H213" s="28">
@@ -10799,7 +10799,7 @@
         <v/>
       </c>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A214" s="9" t="s">
         <v>10</v>
       </c>
@@ -10817,7 +10817,7 @@
       </c>
       <c r="F214" s="22">
         <f>K2*E214</f>
-        <v>257980.83500000002</v>
+        <v>260087.69500000001</v>
       </c>
       <c r="G214" s="22"/>
       <c r="H214" s="10">
@@ -10831,7 +10831,7 @@
         <v/>
       </c>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A215" s="9"/>
       <c r="B215" s="10" t="s">
         <v>503</v>
@@ -10851,7 +10851,7 @@
       <c r="I215" s="12"/>
       <c r="J215" s="1"/>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A216" s="9"/>
       <c r="B216" s="10" t="s">
         <v>504</v>
@@ -10871,7 +10871,7 @@
       <c r="I216" s="12"/>
       <c r="J216" s="1"/>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A217" s="9"/>
       <c r="B217" s="10" t="s">
         <v>505</v>
@@ -10887,7 +10887,7 @@
       </c>
       <c r="F217" s="22">
         <f>K2*E217</f>
-        <v>5021.1035000000002</v>
+        <v>5062.1095000000005</v>
       </c>
       <c r="G217" s="22"/>
       <c r="H217" s="10">
@@ -10901,7 +10901,7 @@
         <v/>
       </c>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A218" s="9"/>
       <c r="B218" s="10" t="s">
         <v>505</v>
@@ -10917,7 +10917,7 @@
       </c>
       <c r="F218" s="22">
         <f>K2*E218</f>
-        <v>5021.1035000000002</v>
+        <v>5062.1095000000005</v>
       </c>
       <c r="G218" s="22"/>
       <c r="H218" s="10">
@@ -10931,7 +10931,7 @@
         <v/>
       </c>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A219" s="9"/>
       <c r="B219" s="10" t="s">
         <v>509</v>
@@ -10957,7 +10957,7 @@
         <v/>
       </c>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A220" s="9"/>
       <c r="B220" s="10" t="s">
         <v>512</v>
@@ -10973,7 +10973,7 @@
       </c>
       <c r="F220" s="22">
         <f>K2*E220</f>
-        <v>29434.055</v>
+        <v>29674.435000000001</v>
       </c>
       <c r="G220" s="22"/>
       <c r="H220" s="10">
@@ -10987,7 +10987,7 @@
         <v/>
       </c>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A221" s="9" t="s">
         <v>10</v>
       </c>
@@ -11005,7 +11005,7 @@
       </c>
       <c r="F221" s="22">
         <f>K2*E221</f>
-        <v>20282.29</v>
+        <v>20447.93</v>
       </c>
       <c r="G221" s="22"/>
       <c r="H221" s="10">
@@ -11019,7 +11019,7 @@
         <v/>
       </c>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A222" s="9" t="s">
         <v>19</v>
       </c>
@@ -11037,7 +11037,7 @@
       </c>
       <c r="F222" s="22">
         <f>K2*E222</f>
-        <v>9339.7471999999998</v>
+        <v>9416.0223999999998</v>
       </c>
       <c r="G222" s="22"/>
       <c r="H222" s="11">
@@ -11051,7 +11051,7 @@
         <v/>
       </c>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A223" s="9" t="s">
         <v>19</v>
       </c>
@@ -11069,7 +11069,7 @@
       </c>
       <c r="F223" s="22">
         <f>K2*E223</f>
-        <v>3977.3076000000001</v>
+        <v>4009.7892000000002</v>
       </c>
       <c r="G223" s="22"/>
       <c r="H223" s="11">
@@ -11083,7 +11083,7 @@
         <v/>
       </c>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A224" s="9" t="s">
         <v>19</v>
       </c>
@@ -11101,7 +11101,7 @@
       </c>
       <c r="F224" s="22">
         <f>K2*E224</f>
-        <v>911.31791800000008</v>
+        <v>918.7604060000001</v>
       </c>
       <c r="G224" s="22"/>
       <c r="H224" s="10">
@@ -11115,7 +11115,7 @@
         <v/>
       </c>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A225" s="9"/>
       <c r="B225" s="10" t="s">
         <v>526</v>
@@ -11131,7 +11131,7 @@
       </c>
       <c r="F225" s="22">
         <f>K2*E225</f>
-        <v>28395.206000000002</v>
+        <v>28627.102000000003</v>
       </c>
       <c r="G225" s="22"/>
       <c r="H225" s="10">
@@ -11145,7 +11145,7 @@
         <v/>
       </c>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A226" s="9"/>
       <c r="B226" s="10" t="s">
         <v>528</v>
@@ -11161,7 +11161,7 @@
       </c>
       <c r="F226" s="22">
         <f>K2*E226</f>
-        <v>48850.637500000004</v>
+        <v>49249.587500000001</v>
       </c>
       <c r="G226" s="22"/>
       <c r="H226" s="10">
@@ -11175,7 +11175,7 @@
         <v/>
       </c>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A227" s="9"/>
       <c r="B227" s="10" t="s">
         <v>530</v>
@@ -11191,7 +11191,7 @@
       </c>
       <c r="F227" s="22">
         <f>K2*E227</f>
-        <v>137375.16565500002</v>
+        <v>138497.071635</v>
       </c>
       <c r="G227" s="22"/>
       <c r="H227" s="10">
@@ -11205,7 +11205,7 @@
         <v/>
       </c>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A228" s="9"/>
       <c r="B228" s="10" t="s">
         <v>530</v>
@@ -11233,7 +11233,7 @@
         <v/>
       </c>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A229" s="9"/>
       <c r="B229" s="10" t="s">
         <v>535</v>
@@ -11249,7 +11249,7 @@
       </c>
       <c r="F229" s="22">
         <f>K2*E229</f>
-        <v>85099.096718999994</v>
+        <v>85794.078122999999</v>
       </c>
       <c r="G229" s="22"/>
       <c r="H229" s="10">
@@ -11263,7 +11263,7 @@
         <v/>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A230" s="9"/>
       <c r="B230" s="10" t="s">
         <v>539</v>
@@ -11279,7 +11279,7 @@
       </c>
       <c r="F230" s="22">
         <f>K2*E230</f>
-        <v>137370.46610000002</v>
+        <v>138492.33370000002</v>
       </c>
       <c r="G230" s="22"/>
       <c r="H230" s="10">
@@ -11293,7 +11293,7 @@
         <v/>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A231" s="9"/>
       <c r="B231" s="10" t="s">
         <v>542</v>
@@ -11309,7 +11309,7 @@
       </c>
       <c r="F231" s="22">
         <f>K2*E231</f>
-        <v>5345.3727950000002</v>
+        <v>5389.0270149999997</v>
       </c>
       <c r="G231" s="22"/>
       <c r="H231" s="10">
@@ -11323,7 +11323,7 @@
         <v/>
       </c>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A232" s="9"/>
       <c r="B232" s="10" t="s">
         <v>544</v>
@@ -11339,7 +11339,7 @@
       </c>
       <c r="F232" s="22">
         <f>K2*E232</f>
-        <v>634.43992500000002</v>
+        <v>639.62122499999998</v>
       </c>
       <c r="G232" s="22"/>
       <c r="H232" s="10">
@@ -11353,7 +11353,7 @@
         <v/>
       </c>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A233" s="9"/>
       <c r="B233" s="10" t="s">
         <v>544</v>
@@ -11381,7 +11381,7 @@
         <v/>
       </c>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A234" s="9"/>
       <c r="B234" s="10" t="s">
         <v>548</v>
@@ -11404,7 +11404,7 @@
         <v/>
       </c>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A235" s="9"/>
       <c r="B235" s="10" t="s">
         <v>550</v>
@@ -11430,7 +11430,7 @@
         <v/>
       </c>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A236" s="9" t="s">
         <v>10</v>
       </c>
@@ -11455,7 +11455,7 @@
       <c r="I236" s="12"/>
       <c r="J236" s="1"/>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A237" s="9"/>
       <c r="B237" s="105" t="s">
         <v>86</v>
@@ -11478,7 +11478,7 @@
       <c r="I237" s="12"/>
       <c r="J237" s="1"/>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A238" s="9"/>
       <c r="B238" s="105" t="s">
         <v>553</v>
@@ -11499,7 +11499,7 @@
       <c r="I238" s="12"/>
       <c r="J238" s="1"/>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A239" s="9"/>
       <c r="B239" s="105" t="s">
         <v>555</v>
@@ -11522,7 +11522,7 @@
       <c r="I239" s="12"/>
       <c r="J239" s="1"/>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A240" s="9"/>
       <c r="B240" s="105" t="s">
         <v>555</v>
@@ -11545,7 +11545,7 @@
       <c r="I240" s="12"/>
       <c r="J240" s="1"/>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A241" s="9"/>
       <c r="B241" s="105" t="s">
         <v>558</v>
@@ -11568,7 +11568,7 @@
       <c r="I241" s="12"/>
       <c r="J241" s="1"/>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A242" s="9"/>
       <c r="B242" s="105" t="s">
         <v>559</v>
@@ -11591,7 +11591,7 @@
       <c r="I242" s="12"/>
       <c r="J242" s="1"/>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A243" s="9"/>
       <c r="B243" s="105" t="s">
         <v>559</v>
@@ -11614,7 +11614,7 @@
       <c r="I243" s="12"/>
       <c r="J243" s="1"/>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A244" s="9"/>
       <c r="B244" s="105" t="s">
         <v>530</v>
@@ -11638,7 +11638,7 @@
       <c r="I244" s="12"/>
       <c r="J244" s="1"/>
     </row>
-    <row r="245" spans="1:10">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A245" s="9" t="s">
         <v>19</v>
       </c>
@@ -11662,7 +11662,7 @@
       <c r="I245" s="12"/>
       <c r="J245" s="1"/>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A246" s="9" t="s">
         <v>19</v>
       </c>
@@ -11686,7 +11686,7 @@
       <c r="I246" s="12"/>
       <c r="J246" s="1"/>
     </row>
-    <row r="247" spans="1:10">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A247" s="9" t="s">
         <v>10</v>
       </c>
@@ -11710,7 +11710,7 @@
       <c r="I247" s="12"/>
       <c r="J247" s="1"/>
     </row>
-    <row r="248" spans="1:10">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A248" s="9" t="s">
         <v>10</v>
       </c>
@@ -11734,7 +11734,7 @@
       <c r="I248" s="12"/>
       <c r="J248" s="1"/>
     </row>
-    <row r="249" spans="1:10">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A249" s="9" t="s">
         <v>19</v>
       </c>
@@ -11758,7 +11758,7 @@
       <c r="I249" s="12"/>
       <c r="J249" s="1"/>
     </row>
-    <row r="250" spans="1:10">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A250" s="9" t="s">
         <v>19</v>
       </c>
@@ -11782,7 +11782,7 @@
       <c r="I250" s="12"/>
       <c r="J250" s="1"/>
     </row>
-    <row r="251" spans="1:10">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A251" s="9" t="s">
         <v>19</v>
       </c>
@@ -11806,7 +11806,7 @@
       <c r="I251" s="12"/>
       <c r="J251" s="1"/>
     </row>
-    <row r="252" spans="1:10">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A252" s="9" t="s">
         <v>19</v>
       </c>
@@ -11830,7 +11830,7 @@
       <c r="I252" s="12"/>
       <c r="J252" s="1"/>
     </row>
-    <row r="253" spans="1:10">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A253" s="9" t="s">
         <v>19</v>
       </c>
@@ -11854,7 +11854,7 @@
       <c r="I253" s="12"/>
       <c r="J253" s="1"/>
     </row>
-    <row r="254" spans="1:10">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A254" s="9" t="s">
         <v>19</v>
       </c>
@@ -11878,7 +11878,7 @@
       <c r="I254" s="12"/>
       <c r="J254" s="1"/>
     </row>
-    <row r="255" spans="1:10">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A255" s="9" t="s">
         <v>19</v>
       </c>
@@ -11902,7 +11902,7 @@
       <c r="I255" s="12"/>
       <c r="J255" s="1"/>
     </row>
-    <row r="256" spans="1:10">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A256" s="9" t="s">
         <v>19</v>
       </c>
@@ -11926,7 +11926,7 @@
       <c r="I256" s="12"/>
       <c r="J256" s="1"/>
     </row>
-    <row r="257" spans="1:10">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A257" s="15" t="s">
         <v>19</v>
       </c>
@@ -11950,7 +11950,7 @@
       <c r="I257" s="12"/>
       <c r="J257" s="1"/>
     </row>
-    <row r="258" spans="1:10">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A258" s="15" t="s">
         <v>19</v>
       </c>
@@ -11968,7 +11968,7 @@
       </c>
       <c r="F258" s="22">
         <f>E258*K$2</f>
-        <v>69395.113200000007</v>
+        <v>69961.844400000002</v>
       </c>
       <c r="G258" s="22"/>
       <c r="H258" s="16">
@@ -11977,7 +11977,7 @@
       <c r="I258" s="12"/>
       <c r="J258" s="1"/>
     </row>
-    <row r="259" spans="1:10">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A259" s="15"/>
       <c r="B259" s="10" t="s">
         <v>586</v>
@@ -11997,7 +11997,7 @@
       <c r="I259" s="12"/>
       <c r="J259" s="1"/>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A260" s="15" t="s">
         <v>19</v>
       </c>
@@ -12021,7 +12021,7 @@
       <c r="I260" s="12"/>
       <c r="J260" s="1"/>
     </row>
-    <row r="261" spans="1:10">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A261" s="15"/>
       <c r="B261" s="10" t="s">
         <v>592</v>
@@ -12041,7 +12041,7 @@
       <c r="I261" s="12"/>
       <c r="J261" s="1"/>
     </row>
-    <row r="262" spans="1:10">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A262" s="15"/>
       <c r="B262" s="10" t="s">
         <v>595</v>
@@ -12061,7 +12061,7 @@
       <c r="I262" s="12"/>
       <c r="J262" s="1"/>
     </row>
-    <row r="263" spans="1:10">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A263" s="15"/>
       <c r="B263" s="10" t="s">
         <v>597</v>
@@ -12081,7 +12081,7 @@
       <c r="I263" s="12"/>
       <c r="J263" s="1"/>
     </row>
-    <row r="264" spans="1:10">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A264" s="15"/>
       <c r="B264" s="10" t="s">
         <v>599</v>
@@ -12101,7 +12101,7 @@
       <c r="I264" s="12"/>
       <c r="J264" s="1"/>
     </row>
-    <row r="265" spans="1:10">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A265" s="15"/>
       <c r="B265" s="10" t="s">
         <v>601</v>
@@ -12121,7 +12121,7 @@
       <c r="I265" s="12"/>
       <c r="J265" s="1"/>
     </row>
-    <row r="266" spans="1:10">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A266" s="15"/>
       <c r="B266" s="10" t="s">
         <v>603</v>
@@ -12141,7 +12141,7 @@
       <c r="I266" s="12"/>
       <c r="J266" s="1"/>
     </row>
-    <row r="267" spans="1:10">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A267" s="15"/>
       <c r="B267" s="10" t="s">
         <v>606</v>
@@ -12161,7 +12161,7 @@
       <c r="I267" s="12"/>
       <c r="J267" s="1"/>
     </row>
-    <row r="268" spans="1:10">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A268" s="15" t="s">
         <v>19</v>
       </c>
@@ -12185,7 +12185,7 @@
       <c r="I268" s="12"/>
       <c r="J268" s="1"/>
     </row>
-    <row r="269" spans="1:10">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A269" s="9" t="s">
         <v>19</v>
       </c>
@@ -12211,7 +12211,7 @@
       </c>
       <c r="J269" s="1"/>
     </row>
-    <row r="270" spans="1:10">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A270" s="9" t="s">
         <v>19</v>
       </c>
@@ -12231,7 +12231,7 @@
       <c r="I270" s="12"/>
       <c r="J270" s="1"/>
     </row>
-    <row r="271" spans="1:10">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A271" s="9" t="s">
         <v>19</v>
       </c>
@@ -12251,7 +12251,7 @@
       <c r="I271" s="12"/>
       <c r="J271" s="1"/>
     </row>
-    <row r="272" spans="1:10">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A272" s="9" t="s">
         <v>19</v>
       </c>
@@ -12271,7 +12271,7 @@
       <c r="I272" s="12"/>
       <c r="J272" s="1"/>
     </row>
-    <row r="273" spans="1:10">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A273" s="9"/>
       <c r="B273" s="10" t="s">
         <v>617</v>
@@ -12291,7 +12291,7 @@
       <c r="I273" s="12"/>
       <c r="J273" s="1"/>
     </row>
-    <row r="274" spans="1:10">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A274" s="9"/>
       <c r="B274" s="10" t="s">
         <v>620</v>
@@ -12311,7 +12311,7 @@
       <c r="I274" s="12"/>
       <c r="J274" s="1"/>
     </row>
-    <row r="275" spans="1:10">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A275" s="9"/>
       <c r="B275" s="10" t="s">
         <v>623</v>
@@ -12331,7 +12331,7 @@
       <c r="I275" s="12"/>
       <c r="J275" s="1"/>
     </row>
-    <row r="276" spans="1:10">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A276" s="9"/>
       <c r="B276" s="10" t="s">
         <v>626</v>
@@ -12351,7 +12351,7 @@
       <c r="I276" s="12"/>
       <c r="J276" s="1"/>
     </row>
-    <row r="277" spans="1:10">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A277" s="9"/>
       <c r="B277" s="10" t="s">
         <v>628</v>
@@ -12371,7 +12371,7 @@
       <c r="I277" s="12"/>
       <c r="J277" s="1"/>
     </row>
-    <row r="278" spans="1:10">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A278" s="9"/>
       <c r="B278" s="10" t="s">
         <v>630</v>
@@ -12391,7 +12391,7 @@
       <c r="I278" s="12"/>
       <c r="J278" s="1"/>
     </row>
-    <row r="279" spans="1:10">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A279" s="9"/>
       <c r="B279" s="10" t="s">
         <v>632</v>
@@ -12411,7 +12411,7 @@
       <c r="I279" s="12"/>
       <c r="J279" s="1"/>
     </row>
-    <row r="280" spans="1:10">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A280" s="9"/>
       <c r="B280" s="10" t="s">
         <v>634</v>
@@ -12433,7 +12433,7 @@
       </c>
       <c r="J280" s="1"/>
     </row>
-    <row r="281" spans="1:10">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A281" s="15"/>
       <c r="B281" s="16" t="s">
         <v>636</v>
@@ -12455,7 +12455,7 @@
       </c>
       <c r="J281" s="1"/>
     </row>
-    <row r="282" spans="1:10">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H282"/>
     </row>
   </sheetData>
@@ -12657,13 +12657,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A39A6148-E43A-4965-9F4A-36C6D678ED00}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A39A6148-E43A-4965-9F4A-36C6D678ED00}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06A72F3A-2E1B-4504-BDC9-0E7BD16E0A51}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06A72F3A-2E1B-4504-BDC9-0E7BD16E0A51}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E087F51-19FF-4963-A285-7904E9E27340}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E087F51-19FF-4963-A285-7904E9E27340}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5fcf6e91-9d2c-4fbe-b73e-6e1cc1240b3e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>